<commit_message>
Avanço na criação da primeira tabela financeira simples
</commit_message>
<xml_diff>
--- a/tabela-financeira/tabela-financeira-simples.xlsx
+++ b/tabela-financeira/tabela-financeira-simples.xlsx
@@ -8,27 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\projetos-excel\tabela-financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DDD59A-5665-4038-9A74-6FD9228382BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C95F64-9738-4188-B9AF-0E262A69AB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{2C3E1D52-378C-46A2-A1F3-936C1DE77944}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2C3E1D52-378C-46A2-A1F3-936C1DE77944}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha" sheetId="1" r:id="rId1"/>
     <sheet name="Auxiliar" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Alimentação">Auxiliar!$D$5:$K$5</definedName>
-    <definedName name="Categorias">Auxiliar!$C$2:$C$7</definedName>
-    <definedName name="Despezas">Planilha!$I$4:$I$31</definedName>
-    <definedName name="Estudos">Auxiliar!$D$3:$K$3</definedName>
+    <definedName name="Alimentação">Auxiliar!$C$5:$J$5</definedName>
+    <definedName name="Categorias">Auxiliar!$B$2:$B$7</definedName>
+    <definedName name="Despezas">Planilha!$H$4:$H$31</definedName>
+    <definedName name="Estudos">Auxiliar!$C$3:$J$3</definedName>
     <definedName name="gastosCategorias">Planilha!$F$4:$F$31</definedName>
     <definedName name="gastosSubcategorias">Planilha!$G$4:$G$31</definedName>
-    <definedName name="Lazer">Auxiliar!$D$4:$K$4</definedName>
-    <definedName name="metodosPagamento">Auxiliar!$A$2:$A$5</definedName>
-    <definedName name="Moradia">Auxiliar!$D$2:$K$2</definedName>
-    <definedName name="Saúde">Auxiliar!$D$7:$K$7</definedName>
-    <definedName name="Transporte">Auxiliar!$D$6:$K$6</definedName>
-    <definedName name="Trânsporte">Auxiliar!$D$6:$K$6</definedName>
+    <definedName name="Lazer">Auxiliar!$C$4:$J$4</definedName>
+    <definedName name="metodosPagamento">Auxiliar!#REF!</definedName>
+    <definedName name="Moradia">Auxiliar!$C$2:$J$2</definedName>
+    <definedName name="Saúde">Auxiliar!$C$7:$J$7</definedName>
+    <definedName name="Transporte">Auxiliar!$C$6:$J$6</definedName>
+    <definedName name="Trânsporte">Auxiliar!$C$6:$J$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,48 +50,49 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>Descrição</t>
   </si>
   <si>
-    <t>Método de pagamento</t>
-  </si>
-  <si>
     <t>Valor</t>
   </si>
   <si>
     <t>Categoria</t>
   </si>
   <si>
-    <t>Guardado</t>
-  </si>
-  <si>
     <t>Entrada</t>
   </si>
   <si>
     <t>Saída</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Relação de gastos</t>
   </si>
   <si>
-    <t>Métodos de pagamento</t>
-  </si>
-  <si>
-    <t>Pix</t>
-  </si>
-  <si>
-    <t>Crédito</t>
-  </si>
-  <si>
-    <t>Débito</t>
-  </si>
-  <si>
     <t>Gastos por categoria</t>
   </si>
   <si>
@@ -203,10 +204,31 @@
     <t>Cursos</t>
   </si>
   <si>
-    <t>Dinheiro</t>
-  </si>
-  <si>
-    <t>Mês</t>
+    <t>Inicial</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Gastos por subcategoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mês: </t>
+  </si>
+  <si>
+    <t>Comida</t>
+  </si>
+  <si>
+    <t>Dia de comer</t>
+  </si>
+  <si>
+    <t>Gastos por subcategorias</t>
+  </si>
+  <si>
+    <t>Jantinha</t>
+  </si>
+  <si>
+    <t>Sopa pa nóis</t>
   </si>
 </sst>
 </file>
@@ -241,19 +263,18 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="18"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <color theme="3"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -264,7 +285,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -359,39 +380,38 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -401,95 +421,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título" xfId="2" builtinId="15"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -526,7 +482,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha!$L$3</c:f>
+              <c:f>Planilha!$K$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -545,7 +501,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -565,7 +521,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -574,29 +530,34 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3D9A-4CBA-A471-EDD646F0B1C0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strLit>
               <c:ptCount val="2"/>
               <c:pt idx="0">
-                <c:v>Gastos</c:v>
+                <c:v>Final</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>Restante</c:v>
+                <c:v>Saída</c:v>
               </c:pt>
             </c:strLit>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Planilha!$B$12,Planilha!$B$16)</c:f>
+              <c:f>(Planilha!$B$16,Planilha!$B$12)</c:f>
               <c:numCache>
                 <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>767</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>990</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,7 +663,1162 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17484566744145361"/>
+          <c:y val="1.5156216435544311E-2"/>
+          <c:w val="0.65427632401089697"/>
+          <c:h val="0.31241198653841562"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha!$K$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gastos por categoria</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:explosion val="2"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Auxiliar!$L$2:$L$27</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>Água</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Luz</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gás</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Aluguel</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Financiamento</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>IPTU</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Internet</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Condomínio</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Livros</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cursos</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Compras</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Cinema</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Streaming</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Videogames</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Compras do mês</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Delivery</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Restaurante</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>IPVA</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Financiamento</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Gasolina</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Transporte público</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Aplicativos de viagem</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Convênio médico</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Academia</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Convênio odontológico</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Medicamentos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Auxiliar!$M$2:$M$27</c:f>
+              <c:numCache>
+                <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0514-4D5A-BED3-E23365B7E2AB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.1747956811876737E-2"/>
+          <c:y val="0.32937188223500491"/>
+          <c:w val="0.92036386909630152"/>
+          <c:h val="0.5455852970227808"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha!$K$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gastos por categoria</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Auxiliar!$O$2:$O$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Moradia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Estudos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lazer</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Alimentação</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Transporte</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Saúde</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Auxiliar!$P$2:$P$7</c:f>
+              <c:numCache>
+                <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7399-4017-AA72-114EEBD13269}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1261,17 +2377,1055 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>4646</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>18934</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>9292</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -1299,17 +3453,79 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>612320</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92052A59-6844-B766-712C-A315A74DC3BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>599514</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>77320</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DCC391E-09CB-4E4F-3E43-AA8A6DEC0E5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7930AB6D-1AEB-45D2-A719-2A2178A06FE6}" name="Tabela2" displayName="Tabela2" ref="A1:A5" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
-  <autoFilter ref="A1:A5" xr:uid="{7930AB6D-1AEB-45D2-A719-2A2178A06FE6}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2ACEA4CB-1968-439A-A774-BD3DEDD1A85E}" name="Métodos de pagamento" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1633,370 +3849,354 @@
     <tabColor theme="4" tint="0.59999389629810485"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B1:L31"/>
+  <dimension ref="B1:M31"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="34.140625" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="31.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="44.140625" customWidth="1"/>
+    <col min="13" max="13" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="D1" s="17" t="s">
+    <row r="1" spans="2:13" ht="24" x14ac:dyDescent="0.4">
+      <c r="D1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="3" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>490</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="4">
+        <v>100</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="14">
-        <v>490</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="1"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="1"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="5">
+        <v>123</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="1"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>5</v>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="1"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="H7" s="4"/>
+      <c r="I7" s="1"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
         <v>500</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="1"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="1"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="1"/>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H9" s="4"/>
+      <c r="I9" s="1"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>6</v>
+      <c r="H10" s="4"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="1"/>
-      <c r="L11" s="19"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="15">
+      <c r="H11" s="4"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
         <f>SUM(Despezas)</f>
-        <v>0</v>
+        <v>223</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="1"/>
-      <c r="L12" s="19"/>
-    </row>
-    <row r="13" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="1"/>
-      <c r="L13" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="4"/>
+      <c r="I13" s="1"/>
+      <c r="K13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="1"/>
-      <c r="L14" s="19"/>
-    </row>
-    <row r="15" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>7</v>
+      <c r="H14" s="4"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="15">
+      <c r="H15" s="4"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
         <f>SUM(B4,B8)-B12</f>
-        <v>990</v>
+        <v>767</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="1"/>
-      <c r="L16" s="19"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H17" s="4"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="4"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="4"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H20" s="4"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="4"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="4"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="4"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="4"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="4"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="4"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H27" s="4"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="4"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="4"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="4"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="1"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K4:K9"/>
+    <mergeCell ref="D1:I1"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="L4:L9"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H31" xr:uid="{44DA035A-2C5F-4684-82F0-4D21A5D7EC01}">
-      <formula1>metodosPagamento</formula1>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F31" xr:uid="{64754CA2-385D-499F-9DE5-C78DF6A91538}">
       <formula1>Categorias</formula1>
     </dataValidation>
@@ -2015,191 +4215,450 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="B1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13"/>
+      <c r="L1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="17"/>
+      <c r="O1" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="19"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="10"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4" cm="1">
+        <f t="array" ref="M2">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L2))</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="4" cm="1">
+        <f t="array" ref="P2">SUMPRODUCT(Despezas * (gastosCategorias = Auxiliar!O2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="L3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="4" cm="1">
+        <f t="array" ref="M3">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L3))</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="4" cm="1">
+        <f t="array" ref="P3">SUMPRODUCT(Despezas * (gastosCategorias = Auxiliar!O3))</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="4" cm="1">
+        <f t="array" ref="M4">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L4))</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="4" cm="1">
+        <f t="array" ref="P4">SUMPRODUCT(Despezas * (gastosCategorias = Auxiliar!O4))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>50</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="4" cm="1">
+        <f t="array" ref="M5">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L5))</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="4" cm="1">
+        <f t="array" ref="P5">SUMPRODUCT(Despezas * (gastosCategorias = Auxiliar!O5))</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="4" cm="1">
+        <f t="array" ref="M6">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L6))</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="4" cm="1">
+        <f t="array" ref="P6">SUMPRODUCT(Despezas * (gastosCategorias = Auxiliar!O6))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="4" cm="1">
+        <f t="array" ref="M7">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L7))</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="4" cm="1">
+        <f t="array" ref="P7">SUMPRODUCT(Despezas * (gastosCategorias = Auxiliar!O7))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="4" cm="1">
+        <f t="array" ref="M8">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L8))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="4" cm="1">
+        <f t="array" ref="M9">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L9))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="4" cm="1">
+        <f t="array" ref="M10">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L10))</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" s="4" cm="1">
+        <f t="array" ref="M11">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L11))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="4" cm="1">
+        <f t="array" ref="M12">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L12))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="4" cm="1">
+        <f t="array" ref="M13">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L13))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="4" cm="1">
+        <f t="array" ref="M14">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L14))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="4" cm="1">
+        <f t="array" ref="M15">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L15))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" s="4" cm="1">
+        <f t="array" ref="M16">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L16))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="4" cm="1">
+        <f t="array" ref="M17">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L17))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="4" cm="1">
+        <f t="array" ref="M18">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L18))</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="4" cm="1">
+        <f t="array" ref="M19">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="4" cm="1">
+        <f t="array" ref="M20">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L20))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="4" cm="1">
+        <f t="array" ref="M21">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L21))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22" s="4" cm="1">
+        <f t="array" ref="M22">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L22))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M23" s="4" cm="1">
+        <f t="array" ref="M23">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L23))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M24" s="4" cm="1">
+        <f t="array" ref="M24">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L24))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="4" cm="1">
+        <f t="array" ref="M25">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L25))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="4" cm="1">
+        <f t="array" ref="M26">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L26))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M27" s="4" cm="1">
+        <f t="array" ref="M27">SUMPRODUCT(Despezas * (gastosSubcategorias=Auxiliar!L27))</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:K1"/>
+  <mergeCells count="3">
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>